<commit_message>
end of the day update
</commit_message>
<xml_diff>
--- a/Noise_Calculations.xlsx
+++ b/Noise_Calculations.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\Documents\TUD\DSE\sinkorporated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E45BE1F-8B33-4C1B-B729-6FB7ACB86C15}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEEC07E-7767-4DE3-A5DB-6363C976E098}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="13032" windowHeight="11700" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="6 bladed propeller" sheetId="1" r:id="rId1"/>
     <sheet name="8 bladed propeller" sheetId="3" r:id="rId2"/>
     <sheet name="Approach Aquila" sheetId="2" r:id="rId3"/>
-    <sheet name="Approach" sheetId="7" r:id="rId4"/>
-    <sheet name="Fly-over Aquila" sheetId="5" r:id="rId5"/>
-    <sheet name="Approach ATR 72" sheetId="4" r:id="rId6"/>
-    <sheet name="Fly-over ATR 72" sheetId="6" r:id="rId7"/>
+    <sheet name="Frequency" sheetId="8" r:id="rId4"/>
+    <sheet name="Approach" sheetId="7" r:id="rId5"/>
+    <sheet name="Fly-over Aquila" sheetId="5" r:id="rId6"/>
+    <sheet name="Approach ATR 72" sheetId="4" r:id="rId7"/>
+    <sheet name="Fly-over ATR 72" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="174">
   <si>
     <t>Propeller noise prediction (empirical)</t>
   </si>
@@ -2178,7 +2179,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-4C7D-4FF5-AB21-5B4ADCBC0459}"/>
                   </c:ext>
@@ -4047,7 +4048,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-9AD0-4FB4-ACA5-90D1BE054A8F}"/>
                   </c:ext>
@@ -5916,7 +5917,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-6DB5-4822-B2C1-70A727BBDCF8}"/>
                   </c:ext>
@@ -7785,7 +7786,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-7D14-4AAF-8BB3-D9AB3BDBABB6}"/>
                   </c:ext>
@@ -16355,10 +16356,1918 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7410C29A-0EEA-4B62-B692-9F42C338054E}">
+  <dimension ref="A1:P30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I1" t="s">
+        <v>139</v>
+      </c>
+      <c r="J1" t="s">
+        <v>140</v>
+      </c>
+      <c r="K1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M1" t="s">
+        <v>144</v>
+      </c>
+      <c r="N1" t="s">
+        <v>147</v>
+      </c>
+      <c r="O1" t="s">
+        <v>146</v>
+      </c>
+      <c r="P1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H2" t="s">
+        <v>138</v>
+      </c>
+      <c r="J2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L2" t="s">
+        <v>143</v>
+      </c>
+      <c r="N2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <f ca="1">(A3*$F$10*(1-$B$7*COS($B$14)))/($B$7*$B$9)</f>
+        <v>1.3712518425477178E-3</v>
+      </c>
+      <c r="C3">
+        <f ca="1">10*LOG10((($B$12*$B$9*$F$11*$F$14*(0.613*(10*B3)^4*((10*B3)^1.5+0.5)^-4))/(4*PI()*$B$15^2*(1-$B$7*COS($B$14))))/$B$17^2)</f>
+        <v>61.705215447311737</v>
+      </c>
+      <c r="D3">
+        <f ca="1">(A3*$H$10)*(1-$B$7*COS($B$14))/($B$7*$B$9)</f>
+        <v>8.5335278096141813E-5</v>
+      </c>
+      <c r="E3">
+        <f ca="1">10*LOG10((($B$12*$B$9*$H$16*$H$15*(0.613*(10*D3)^4*((10*D3)^1.5+0.5)^-4))/(4*PI()*$B$15^2*(1-$B$7*COS($B$14))^4))/$B$17^2)</f>
+        <v>7.7631670509020836</v>
+      </c>
+      <c r="F3">
+        <f ca="1">(A3*$J$10)*(1-$B$7*COS($B$14))/($B$7*$B$9)</f>
+        <v>2.8457121976312215E-5</v>
+      </c>
+      <c r="G3">
+        <f ca="1">10*LOG10((($B$12*$B$9*$J$16*$J$15*(0.613*(10*F3)^4*((10*F3)^1.5+0.5)^-4))/(4*PI()*$B$15^2*(1-$B$7*COS($B$14))^4))/$B$17^2)</f>
+        <v>-52.885279001976137</v>
+      </c>
+      <c r="H3">
+        <f ca="1">(A3*$F$25)*(1-$B$7*COS($B$14))/($B$7*$B$9)</f>
+        <v>8.8928500693206597E-2</v>
+      </c>
+      <c r="I3">
+        <f ca="1">10*LOG10((($B$12*$B$9*$F$32*$F$31*(0.1406*H3^-0.55))/(4*PI()*$B$15^2*(1-$B$7*COS($B$14))^2))/$B$17^2)</f>
+        <v>134.65693802981943</v>
+      </c>
+      <c r="J3">
+        <f ca="1">(A3*$F$25)*(1-$B$7*COS($B$14))/($B$7*$B$9)</f>
+        <v>8.8928500693206597E-2</v>
+      </c>
+      <c r="K3">
+        <f ca="1">10*LOG10((($B$12*$B$9*$H$31*$H$30*(13.59*J3^2*(J3^2+12.5)^-2.25))/(4*PI()*$B$15^2*(1-$B$7*COS($B$14))^4))/$B$17^2)</f>
+        <v>67.038885476407103</v>
+      </c>
+      <c r="L3">
+        <f ca="1">(A3*$J$27)*(1-$B$7*COS($B$14))/($B$7*$B$9)</f>
+        <v>3.9215686274509803E-2</v>
+      </c>
+      <c r="M3">
+        <f ca="1">10*LOG10((($B$12*$B$9*$F$32*$F$31*(13.59*L3^2*(L3^2+12.5)^-2.25))/(4*PI()*$B$15^2*(1-$B$7*COS($B$14))^2))/$B$17^2)</f>
+        <v>95.91652370032817</v>
+      </c>
+      <c r="N3">
+        <f ca="1">(A3*$F$42)*(1-$B$7*COS($B$14))/($B$7*$B$9)</f>
+        <v>6.5359477124183009E-3</v>
+      </c>
+      <c r="O3">
+        <f ca="1">10*LOG10((($B$12*$B$9*$F$46*$F$45*(5.325*(30+N3^8)^-1))/(4*PI()*$B$15^2*(1-$B$7*COS($B$14))^2))/$B$17^2)</f>
+        <v>73.4906225152682</v>
+      </c>
+      <c r="P3">
+        <f ca="1">10*LOG10(10^(C3/10)+10^(E3/10)+10^(G3/10)+10^(I3/10)+10^(K3/10)+10^(M3/10)+10^(O3/10))</f>
+        <v>134.65752270293817</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:B30" ca="1" si="0">(A4*$F$10*(1-$B$7*COS($B$14)))/($B$7*$B$9)</f>
+        <v>2.7425036850954355E-3</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C30" ca="1" si="1">10*LOG10((($B$12*$B$9*$F$11*$F$14*(0.613*(10*B4)^4*((10*B4)^1.5+0.5)^-4))/(4*PI()*$B$15^2*(1-$B$7*COS($B$14))))/$B$17^2)</f>
+        <v>73.645031749520257</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D30" ca="1" si="2">(A4*$H$10)*(1-$B$7*COS($B$14))/($B$7*$B$9)</f>
+        <v>1.7067055619228363E-4</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E29" ca="1" si="3">10*LOG10((($B$12*$B$9*$H$16*$H$15*(0.613*(10*D4)^4*((10*D4)^1.5+0.5)^-4))/(4*PI()*$B$15^2*(1-$B$7*COS($B$14))^4))/$B$17^2)</f>
+        <v>19.802783430865269</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F30" ca="1" si="4">(A4*$J$10)*(1-$B$7*COS($B$14))/($B$7*$B$9)</f>
+        <v>5.6914243952624429E-5</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G30" ca="1" si="5">10*LOG10((($B$12*$B$9*$J$16*$J$15*(0.613*(10*F4)^4*((10*F4)^1.5+0.5)^-4))/(4*PI()*$B$15^2*(1-$B$7*COS($B$14))^4))/$B$17^2)</f>
+        <v>-40.844384126679117</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H30" ca="1" si="6">(A4*$F$25)*(1-$B$7*COS($B$14))/($B$7*$B$9)</f>
+        <v>0.17785700138641319</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I30" ca="1" si="7">10*LOG10((($B$12*$B$9*$F$32*$F$31*(0.1406*H4^-0.55))/(4*PI()*$B$15^2*(1-$B$7*COS($B$14))^2))/$B$17^2)</f>
+        <v>133.00127305366755</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J30" ca="1" si="8">(A4*$F$25)*(1-$B$7*COS($B$14))/($B$7*$B$9)</f>
+        <v>0.17785700138641319</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ref="K4:K30" ca="1" si="9">10*LOG10((($B$12*$B$9*$H$31*$H$30*(13.59*J4^2*(J4^2+12.5)^-2.25))/(4*PI()*$B$15^2*(1-$B$7*COS($B$14))^4))/$B$17^2)</f>
+        <v>73.040968255232144</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L30" ca="1" si="10">(A4*$J$27)*(1-$B$7*COS($B$14))/($B$7*$B$9)</f>
+        <v>7.8431372549019607E-2</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M30" ca="1" si="11">10*LOG10((($B$12*$B$9*$F$32*$F$31*(13.59*L4^2*(L4^2+12.5)^-2.25))/(4*PI()*$B$15^2*(1-$B$7*COS($B$14))^2))/$B$17^2)</f>
+        <v>101.93351812474795</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ref="N4:N30" ca="1" si="12">(A4*$F$42)*(1-$B$7*COS($B$14))/($B$7*$B$9)</f>
+        <v>1.3071895424836602E-2</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O30" ca="1" si="13">10*LOG10((($B$12*$B$9*$F$46*$F$45*(5.325*(30+N4^8)^-1))/(4*PI()*$B$15^2*(1-$B$7*COS($B$14))^2))/$B$17^2)</f>
+        <v>73.4906225152682</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4:P30" ca="1" si="14">10*LOG10(10^(C4/10)+10^(E4/10)+10^(G4/10)+10^(I4/10)+10^(K4/10)+10^(M4/10)+10^(O4/10))</f>
+        <v>133.00468231748386</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.1137555276431533E-3</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ca="1" si="1"/>
+        <v>80.558268424332311</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ca="1" si="2"/>
+        <v>2.5600583428842541E-4</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="3"/>
+        <v>26.844383520254816</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ca="1" si="4"/>
+        <v>8.5371365928936654E-5</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ca="1" si="5"/>
+        <v>-33.801128653733748</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.26678550207961976</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ca="1" si="7"/>
+        <v>132.0327711288613</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.26678550207961976</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ca="1" si="9"/>
+        <v>76.532009310095731</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ca="1" si="10"/>
+        <v>0.11764705882352941</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ca="1" si="11"/>
+        <v>105.44933711249037</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ca="1" si="12"/>
+        <v>1.9607843137254902E-2</v>
+      </c>
+      <c r="O5">
+        <f t="shared" ca="1" si="13"/>
+        <v>73.4906225152682</v>
+      </c>
+      <c r="P5">
+        <f t="shared" ca="1" si="14"/>
+        <v>132.04234744284437</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ca="1" si="0"/>
+        <v>5.4850073701908711E-3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ca="1" si="1"/>
+        <v>85.40263827927113</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ca="1" si="2"/>
+        <v>3.4134111238456725E-4</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ca="1" si="3"/>
+        <v>31.839505375407704</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ca="1" si="4"/>
+        <v>1.1382848790524886E-4</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ca="1" si="5"/>
+        <v>-28.804046803559231</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.35571400277282639</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ca="1" si="7"/>
+        <v>131.34560807751564</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.35571400277282639</v>
+      </c>
+      <c r="K6">
+        <f t="shared" ca="1" si="9"/>
+        <v>78.987848546338299</v>
+      </c>
+      <c r="L6">
+        <f t="shared" ca="1" si="10"/>
+        <v>0.15686274509803921</v>
+      </c>
+      <c r="M6">
+        <f t="shared" ca="1" si="11"/>
+        <v>107.93970937124499</v>
+      </c>
+      <c r="N6">
+        <f t="shared" ca="1" si="12"/>
+        <v>2.6143790849673203E-2</v>
+      </c>
+      <c r="O6">
+        <f t="shared" ca="1" si="13"/>
+        <v>73.490622515268186</v>
+      </c>
+      <c r="P6">
+        <f t="shared" ca="1" si="14"/>
+        <v>131.36552934601218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>50</v>
+      </c>
+      <c r="B7">
+        <f t="shared" ca="1" si="0"/>
+        <v>6.8562592127385889E-3</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ca="1" si="1"/>
+        <v>89.10691006772899</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.2667639048070904E-4</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="3"/>
+        <v>35.713152724983146</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ca="1" si="4"/>
+        <v>1.4228560988156108E-4</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ca="1" si="5"/>
+        <v>-24.928176671996646</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.44464250346603296</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ca="1" si="7"/>
+        <v>130.81260300597134</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.44464250346603296</v>
+      </c>
+      <c r="K7">
+        <f t="shared" ca="1" si="9"/>
+        <v>80.871121790223498</v>
+      </c>
+      <c r="L7">
+        <f t="shared" ca="1" si="10"/>
+        <v>0.19607843137254902</v>
+      </c>
+      <c r="M7">
+        <f t="shared" ca="1" si="11"/>
+        <v>109.8671170570116</v>
+      </c>
+      <c r="N7">
+        <f t="shared" ca="1" si="12"/>
+        <v>3.2679738562091505E-2</v>
+      </c>
+      <c r="O7">
+        <f t="shared" ca="1" si="13"/>
+        <v>73.490622515268015</v>
+      </c>
+      <c r="P7">
+        <f t="shared" ca="1" si="14"/>
+        <v>130.84773877929192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>60</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ca="1" si="0"/>
+        <v>8.2275110552863066E-3</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ca="1" si="1"/>
+        <v>92.085796680223069</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.1201166857685082E-4</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="3"/>
+        <v>38.877358810124385</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ca="1" si="4"/>
+        <v>1.7074273185787331E-4</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ca="1" si="5"/>
+        <v>-21.761513278227479</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.53357100415923953</v>
+      </c>
+      <c r="I8">
+        <f t="shared" ca="1" si="7"/>
+        <v>130.37710615270939</v>
+      </c>
+      <c r="J8">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.53357100415923953</v>
+      </c>
+      <c r="K8">
+        <f t="shared" ca="1" si="9"/>
+        <v>82.388030292627747</v>
+      </c>
+      <c r="L8">
+        <f t="shared" ca="1" si="10"/>
+        <v>0.23529411764705882</v>
+      </c>
+      <c r="M8">
+        <f t="shared" ca="1" si="11"/>
+        <v>111.43756722112039</v>
+      </c>
+      <c r="N8">
+        <f t="shared" ca="1" si="12"/>
+        <v>3.9215686274509803E-2</v>
+      </c>
+      <c r="O8">
+        <f t="shared" ca="1" si="13"/>
+        <v>73.490622515267404</v>
+      </c>
+      <c r="P8">
+        <f t="shared" ca="1" si="14"/>
+        <v>130.43290858624624</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>70</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ca="1" si="0"/>
+        <v>9.5987628978340244E-3</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ca="1" si="1"/>
+        <v>94.561166914686822</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.9734694667299272E-4</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ca="1" si="3"/>
+        <v>41.551921763285392</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ca="1" si="4"/>
+        <v>1.9919985383418554E-4</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ca="1" si="5"/>
+        <v>-19.084279269420637</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.62249950485244621</v>
+      </c>
+      <c r="I9">
+        <f t="shared" ca="1" si="7"/>
+        <v>130.00889880974103</v>
+      </c>
+      <c r="J9">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.62249950485244621</v>
+      </c>
+      <c r="K9">
+        <f t="shared" ca="1" si="9"/>
+        <v>83.648702220421271</v>
+      </c>
+      <c r="L9">
+        <f t="shared" ca="1" si="10"/>
+        <v>0.27450980392156865</v>
+      </c>
+      <c r="M9">
+        <f t="shared" ca="1" si="11"/>
+        <v>112.76095571315837</v>
+      </c>
+      <c r="N9">
+        <f t="shared" ca="1" si="12"/>
+        <v>4.5751633986928102E-2</v>
+      </c>
+      <c r="O9">
+        <f t="shared" ca="1" si="13"/>
+        <v>73.490622515265429</v>
+      </c>
+      <c r="P9">
+        <f t="shared" ca="1" si="14"/>
+        <v>130.09130553165622</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>80</v>
+      </c>
+      <c r="B10">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.0970014740381742E-2</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ca="1" si="1"/>
+        <v>96.665908230728917</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.8268222476913451E-4</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ca="1" si="3"/>
+        <v>43.868046084808938</v>
+      </c>
+      <c r="F10">
+        <f t="shared" ca="1" si="4"/>
+        <v>2.2765697581049772E-4</v>
+      </c>
+      <c r="G10">
+        <f t="shared" ca="1" si="5"/>
+        <v>-16.765286273295594</v>
+      </c>
+      <c r="H10">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.71142800554565278</v>
+      </c>
+      <c r="I10">
+        <f t="shared" ca="1" si="7"/>
+        <v>129.68994310136372</v>
+      </c>
+      <c r="J10">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.71142800554565278</v>
+      </c>
+      <c r="K10">
+        <f t="shared" ca="1" si="9"/>
+        <v>84.719008799665005</v>
+      </c>
+      <c r="L10">
+        <f t="shared" ca="1" si="10"/>
+        <v>0.31372549019607843</v>
+      </c>
+      <c r="M10">
+        <f t="shared" ca="1" si="11"/>
+        <v>113.9028861439327</v>
+      </c>
+      <c r="N10">
+        <f t="shared" ca="1" si="12"/>
+        <v>5.2287581699346407E-2</v>
+      </c>
+      <c r="O10">
+        <f t="shared" ca="1" si="13"/>
+        <v>73.490622515260128</v>
+      </c>
+      <c r="P10">
+        <f t="shared" ca="1" si="14"/>
+        <v>129.80528318598624</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>90</v>
+      </c>
+      <c r="B11">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.2341266582929458E-2</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ca="1" si="1"/>
+        <v>98.486067785463845</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ca="1" si="2"/>
+        <v>7.6801750286527629E-4</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ca="1" si="3"/>
+        <v>45.91036457509415</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ca="1" si="4"/>
+        <v>2.5611409778680995E-4</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ca="1" si="5"/>
+        <v>-14.719914489289245</v>
+      </c>
+      <c r="H11">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.80035650623885923</v>
+      </c>
+      <c r="I11">
+        <f t="shared" ca="1" si="7"/>
+        <v>129.40860422790314</v>
+      </c>
+      <c r="J11">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.80035650623885923</v>
+      </c>
+      <c r="K11">
+        <f t="shared" ca="1" si="9"/>
+        <v>85.641571150936699</v>
+      </c>
+      <c r="L11">
+        <f t="shared" ca="1" si="10"/>
+        <v>0.35294117647058826</v>
+      </c>
+      <c r="M11">
+        <f t="shared" ca="1" si="11"/>
+        <v>114.90567988088371</v>
+      </c>
+      <c r="N11">
+        <f t="shared" ca="1" si="12"/>
+        <v>5.8823529411764705E-2</v>
+      </c>
+      <c r="O11">
+        <f t="shared" ca="1" si="13"/>
+        <v>73.490622515247452</v>
+      </c>
+      <c r="P11">
+        <f t="shared" ca="1" si="14"/>
+        <v>129.56350383189144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>100</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.3712518425477178E-2</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ca="1" si="1"/>
+        <v>100.08065113814754</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ca="1" si="2"/>
+        <v>8.5335278096141808E-4</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ca="1" si="3"/>
+        <v>47.736666260775984</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ca="1" si="4"/>
+        <v>2.8457121976312215E-4</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ca="1" si="5"/>
+        <v>-12.890385666437233</v>
+      </c>
+      <c r="H12">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.88928500693206591</v>
+      </c>
+      <c r="I12">
+        <f t="shared" ca="1" si="7"/>
+        <v>129.15693802981943</v>
+      </c>
+      <c r="J12">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.88928500693206591</v>
+      </c>
+      <c r="K12">
+        <f t="shared" ca="1" si="9"/>
+        <v>86.445620234112766</v>
+      </c>
+      <c r="L12">
+        <f t="shared" ca="1" si="10"/>
+        <v>0.39215686274509803</v>
+      </c>
+      <c r="M12">
+        <f t="shared" ca="1" si="11"/>
+        <v>115.79823942015965</v>
+      </c>
+      <c r="N12">
+        <f t="shared" ca="1" si="12"/>
+        <v>6.535947712418301E-2</v>
+      </c>
+      <c r="O12">
+        <f t="shared" ca="1" si="13"/>
+        <v>73.490622515219997</v>
+      </c>
+      <c r="P12">
+        <f t="shared" ca="1" si="14"/>
+        <v>129.35822489697173</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>200</v>
+      </c>
+      <c r="B13">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.7425036850954355E-2</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ca="1" si="1"/>
+        <v>109.41568128779709</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ca="1" si="2"/>
+        <v>1.7067055619228362E-3</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ca="1" si="3"/>
+        <v>59.727938974122068</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ca="1" si="4"/>
+        <v>5.6914243952624431E-4</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ca="1" si="5"/>
+        <v>-0.85882382164188376</v>
+      </c>
+      <c r="H13">
+        <f t="shared" ca="1" si="6"/>
+        <v>1.7785700138641318</v>
+      </c>
+      <c r="I13">
+        <f t="shared" ca="1" si="7"/>
+        <v>127.50127305366753</v>
+      </c>
+      <c r="J13">
+        <f t="shared" ca="1" si="8"/>
+        <v>1.7785700138641318</v>
+      </c>
+      <c r="K13">
+        <f t="shared" ca="1" si="9"/>
+        <v>90.861260333834224</v>
+      </c>
+      <c r="L13">
+        <f t="shared" ca="1" si="10"/>
+        <v>0.78431372549019607</v>
+      </c>
+      <c r="M13">
+        <f t="shared" ca="1" si="11"/>
+        <v>121.46890411075313</v>
+      </c>
+      <c r="N13">
+        <f t="shared" ca="1" si="12"/>
+        <v>0.13071895424836602</v>
+      </c>
+      <c r="O13">
+        <f t="shared" ca="1" si="13"/>
+        <v>73.490622502926598</v>
+      </c>
+      <c r="P13">
+        <f t="shared" ca="1" si="14"/>
+        <v>128.52246661838817</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>300</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.113755527643153E-2</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ca="1" si="1"/>
+        <v>113.48423373593812</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ca="1" si="2"/>
+        <v>2.5600583428842544E-3</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ca="1" si="3"/>
+        <v>66.707148611431165</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ca="1" si="4"/>
+        <v>8.5371365928936657E-4</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ca="1" si="5"/>
+        <v>6.1723537574626857</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ca="1" si="6"/>
+        <v>2.6678550207961975</v>
+      </c>
+      <c r="I14">
+        <f t="shared" ca="1" si="7"/>
+        <v>126.53277112886128</v>
+      </c>
+      <c r="J14">
+        <f t="shared" ca="1" si="8"/>
+        <v>2.6678550207961975</v>
+      </c>
+      <c r="K14">
+        <f t="shared" ca="1" si="9"/>
+        <v>92.183508368949973</v>
+      </c>
+      <c r="L14">
+        <f t="shared" ca="1" si="10"/>
+        <v>1.1764705882352942</v>
+      </c>
+      <c r="M14">
+        <f t="shared" ca="1" si="11"/>
+        <v>124.43398915294502</v>
+      </c>
+      <c r="N14">
+        <f t="shared" ca="1" si="12"/>
+        <v>0.19607843137254902</v>
+      </c>
+      <c r="O14">
+        <f t="shared" ca="1" si="13"/>
+        <v>73.490622198966435</v>
+      </c>
+      <c r="P14">
+        <f t="shared" ca="1" si="14"/>
+        <v>128.75135333469103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>400</v>
+      </c>
+      <c r="B15">
+        <f t="shared" ca="1" si="0"/>
+        <v>5.4850073701908711E-2</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ca="1" si="1"/>
+        <v>115.51268830439282</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ca="1" si="2"/>
+        <v>3.4134111238456723E-3</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ca="1" si="3"/>
+        <v>71.628695577854046</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ca="1" si="4"/>
+        <v>1.1382848790524886E-3</v>
+      </c>
+      <c r="G15">
+        <f t="shared" ca="1" si="5"/>
+        <v>11.155144591256953</v>
+      </c>
+      <c r="H15">
+        <f t="shared" ca="1" si="6"/>
+        <v>3.5571400277282637</v>
+      </c>
+      <c r="I15">
+        <f t="shared" ca="1" si="7"/>
+        <v>125.84560807751564</v>
+      </c>
+      <c r="J15">
+        <f t="shared" ca="1" si="8"/>
+        <v>3.5571400277282637</v>
+      </c>
+      <c r="K15">
+        <f t="shared" ca="1" si="9"/>
+        <v>92.25337523876847</v>
+      </c>
+      <c r="L15">
+        <f t="shared" ca="1" si="10"/>
+        <v>1.5686274509803921</v>
+      </c>
+      <c r="M15">
+        <f t="shared" ca="1" si="11"/>
+        <v>126.20305336124885</v>
+      </c>
+      <c r="N15">
+        <f t="shared" ca="1" si="12"/>
+        <v>0.26143790849673204</v>
+      </c>
+      <c r="O15">
+        <f t="shared" ca="1" si="13"/>
+        <v>73.490619355818964</v>
+      </c>
+      <c r="P15">
+        <f t="shared" ca="1" si="14"/>
+        <v>129.22789001260801</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>500</v>
+      </c>
+      <c r="B16">
+        <f t="shared" ca="1" si="0"/>
+        <v>6.8562592127385885E-2</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ca="1" si="1"/>
+        <v>116.54029176964529</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.2667639048070902E-3</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ca="1" si="3"/>
+        <v>75.419288788899721</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ca="1" si="4"/>
+        <v>1.4228560988156108E-3</v>
+      </c>
+      <c r="G16">
+        <f t="shared" ca="1" si="5"/>
+        <v>15.014819899074446</v>
+      </c>
+      <c r="H16">
+        <f t="shared" ca="1" si="6"/>
+        <v>4.4464250346603293</v>
+      </c>
+      <c r="I16">
+        <f t="shared" ca="1" si="7"/>
+        <v>125.31260300597133</v>
+      </c>
+      <c r="J16">
+        <f t="shared" ca="1" si="8"/>
+        <v>4.4464250346603293</v>
+      </c>
+      <c r="K16">
+        <f t="shared" ca="1" si="9"/>
+        <v>91.756753690469139</v>
+      </c>
+      <c r="L16">
+        <f t="shared" ca="1" si="10"/>
+        <v>1.9607843137254901</v>
+      </c>
+      <c r="M16">
+        <f t="shared" ca="1" si="11"/>
+        <v>127.27663461828031</v>
+      </c>
+      <c r="N16">
+        <f t="shared" ca="1" si="12"/>
+        <v>0.32679738562091504</v>
+      </c>
+      <c r="O16">
+        <f t="shared" ca="1" si="13"/>
+        <v>73.490603683517207</v>
+      </c>
+      <c r="P16">
+        <f t="shared" ca="1" si="14"/>
+        <v>129.63419203708975</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>600</v>
+      </c>
+      <c r="B17">
+        <f t="shared" ca="1" si="0"/>
+        <v>8.2275110552863059E-2</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ca="1" si="1"/>
+        <v>117.02111864854547</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.1201166857685089E-3</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ca="1" si="3"/>
+        <v>78.49214971511563</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ca="1" si="4"/>
+        <v>1.7074273185787331E-3</v>
+      </c>
+      <c r="G17">
+        <f t="shared" ca="1" si="5"/>
+        <v>18.163594891917455</v>
+      </c>
+      <c r="H17">
+        <f t="shared" ca="1" si="6"/>
+        <v>5.335710041592395</v>
+      </c>
+      <c r="I17">
+        <f t="shared" ca="1" si="7"/>
+        <v>124.8771061527094</v>
+      </c>
+      <c r="J17">
+        <f t="shared" ca="1" si="8"/>
+        <v>5.335710041592395</v>
+      </c>
+      <c r="K17">
+        <f t="shared" ca="1" si="9"/>
+        <v>91.008129080353442</v>
+      </c>
+      <c r="L17">
+        <f t="shared" ca="1" si="10"/>
+        <v>2.3529411764705883</v>
+      </c>
+      <c r="M17">
+        <f t="shared" ca="1" si="11"/>
+        <v>127.89789105842472</v>
+      </c>
+      <c r="N17">
+        <f t="shared" ca="1" si="12"/>
+        <v>0.39215686274509803</v>
+      </c>
+      <c r="O17">
+        <f t="shared" ca="1" si="13"/>
+        <v>73.490541542765172</v>
+      </c>
+      <c r="P17">
+        <f t="shared" ca="1" si="14"/>
+        <v>129.88647632537092</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>700</v>
+      </c>
+      <c r="B18">
+        <f t="shared" ca="1" si="0"/>
+        <v>9.5987628978340248E-2</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ca="1" si="1"/>
+        <v>117.1840441688334</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.9734694667299268E-3</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ca="1" si="3"/>
+        <v>81.067978247555573</v>
+      </c>
+      <c r="F18">
+        <f t="shared" ca="1" si="4"/>
+        <v>1.9919985383418555E-3</v>
+      </c>
+      <c r="G18">
+        <f t="shared" ca="1" si="5"/>
+        <v>20.821402496721831</v>
+      </c>
+      <c r="H18">
+        <f t="shared" ca="1" si="6"/>
+        <v>6.2249950485244616</v>
+      </c>
+      <c r="I18">
+        <f t="shared" ca="1" si="7"/>
+        <v>124.50889880974103</v>
+      </c>
+      <c r="J18">
+        <f t="shared" ca="1" si="8"/>
+        <v>6.2249950485244616</v>
+      </c>
+      <c r="K18">
+        <f t="shared" ca="1" si="9"/>
+        <v>90.159282272778341</v>
+      </c>
+      <c r="L18">
+        <f t="shared" ca="1" si="10"/>
+        <v>2.7450980392156863</v>
+      </c>
+      <c r="M18">
+        <f t="shared" ca="1" si="11"/>
+        <v>128.20962690998965</v>
+      </c>
+      <c r="N18">
+        <f t="shared" ca="1" si="12"/>
+        <v>0.45751633986928103</v>
+      </c>
+      <c r="O18">
+        <f t="shared" ca="1" si="13"/>
+        <v>73.490344606637336</v>
+      </c>
+      <c r="P18">
+        <f t="shared" ca="1" si="14"/>
+        <v>129.9868777088769</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>800</v>
+      </c>
+      <c r="B19">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.10970014740381742</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ca="1" si="1"/>
+        <v>117.15474543343529</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.8268222476913446E-3</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ca="1" si="3"/>
+        <v>83.278701282880348</v>
+      </c>
+      <c r="F19">
+        <f t="shared" ca="1" si="4"/>
+        <v>2.2765697581049772E-3</v>
+      </c>
+      <c r="G19">
+        <f t="shared" ca="1" si="5"/>
+        <v>23.11955266474488</v>
+      </c>
+      <c r="H19">
+        <f t="shared" ca="1" si="6"/>
+        <v>7.1142800554565273</v>
+      </c>
+      <c r="I19">
+        <f t="shared" ca="1" si="7"/>
+        <v>124.18994310136375</v>
+      </c>
+      <c r="J19">
+        <f t="shared" ca="1" si="8"/>
+        <v>7.1142800554565273</v>
+      </c>
+      <c r="K19">
+        <f t="shared" ca="1" si="9"/>
+        <v>89.284670132672304</v>
+      </c>
+      <c r="L19">
+        <f t="shared" ca="1" si="10"/>
+        <v>3.1372549019607843</v>
+      </c>
+      <c r="M19">
+        <f t="shared" ca="1" si="11"/>
+        <v>128.30459370076562</v>
+      </c>
+      <c r="N19">
+        <f t="shared" ca="1" si="12"/>
+        <v>0.52287581699346408</v>
+      </c>
+      <c r="O19">
+        <f t="shared" ca="1" si="13"/>
+        <v>73.489813771274811</v>
+      </c>
+      <c r="P19">
+        <f t="shared" ca="1" si="14"/>
+        <v>129.96188429121889</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>900</v>
+      </c>
+      <c r="B20">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.1234126658292946</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ca="1" si="1"/>
+        <v>117.00640141840621</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ca="1" si="2"/>
+        <v>7.6801750286527625E-3</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ca="1" si="3"/>
+        <v>85.209552277573664</v>
+      </c>
+      <c r="F20">
+        <f t="shared" ca="1" si="4"/>
+        <v>2.5611409778680998E-3</v>
+      </c>
+      <c r="G20">
+        <f t="shared" ca="1" si="5"/>
+        <v>25.142763904501081</v>
+      </c>
+      <c r="H20">
+        <f t="shared" ca="1" si="6"/>
+        <v>8.0035650623885939</v>
+      </c>
+      <c r="I20">
+        <f t="shared" ca="1" si="7"/>
+        <v>123.90860422790314</v>
+      </c>
+      <c r="J20">
+        <f t="shared" ca="1" si="8"/>
+        <v>8.0035650623885939</v>
+      </c>
+      <c r="K20">
+        <f t="shared" ca="1" si="9"/>
+        <v>88.42072388768284</v>
+      </c>
+      <c r="L20">
+        <f t="shared" ca="1" si="10"/>
+        <v>3.5294117647058822</v>
+      </c>
+      <c r="M20">
+        <f t="shared" ca="1" si="11"/>
+        <v>128.24632168044391</v>
+      </c>
+      <c r="N20">
+        <f t="shared" ca="1" si="12"/>
+        <v>0.58823529411764708</v>
+      </c>
+      <c r="O20">
+        <f t="shared" ca="1" si="13"/>
+        <v>73.488547754900765</v>
+      </c>
+      <c r="P20">
+        <f t="shared" ca="1" si="14"/>
+        <v>129.84092070985378</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>1000</v>
+      </c>
+      <c r="B21">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.13712518425477177</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ca="1" si="1"/>
+        <v>116.78350694048127</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ca="1" si="2"/>
+        <v>8.5335278096141803E-3</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ca="1" si="3"/>
+        <v>86.918833341369464</v>
+      </c>
+      <c r="F21">
+        <f t="shared" ca="1" si="4"/>
+        <v>2.8457121976312215E-3</v>
+      </c>
+      <c r="G21">
+        <f t="shared" ca="1" si="5"/>
+        <v>26.948896905236911</v>
+      </c>
+      <c r="H21">
+        <f t="shared" ca="1" si="6"/>
+        <v>8.8928500693206587</v>
+      </c>
+      <c r="I21">
+        <f t="shared" ca="1" si="7"/>
+        <v>123.65693802981943</v>
+      </c>
+      <c r="J21">
+        <f t="shared" ca="1" si="8"/>
+        <v>8.8928500693206587</v>
+      </c>
+      <c r="K21">
+        <f t="shared" ca="1" si="9"/>
+        <v>87.584729697351676</v>
+      </c>
+      <c r="L21">
+        <f t="shared" ca="1" si="10"/>
+        <v>3.9215686274509802</v>
+      </c>
+      <c r="M21">
+        <f t="shared" ca="1" si="11"/>
+        <v>128.07956927702526</v>
+      </c>
+      <c r="N21">
+        <f t="shared" ca="1" si="12"/>
+        <v>0.65359477124183007</v>
+      </c>
+      <c r="O21">
+        <f t="shared" ca="1" si="13"/>
+        <v>73.485804250352331</v>
+      </c>
+      <c r="P21">
+        <f t="shared" ca="1" si="14"/>
+        <v>129.64977816816412</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>2000</v>
+      </c>
+      <c r="B22">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.27425036850954354</v>
+      </c>
+      <c r="C22">
+        <f t="shared" ca="1" si="1"/>
+        <v>113.65774928172884</v>
+      </c>
+      <c r="D22">
+        <f t="shared" ca="1" si="2"/>
+        <v>1.7067055619228361E-2</v>
+      </c>
+      <c r="E22">
+        <f t="shared" ca="1" si="3"/>
+        <v>97.513566001474203</v>
+      </c>
+      <c r="F22">
+        <f t="shared" ca="1" si="4"/>
+        <v>5.6914243952624431E-3</v>
+      </c>
+      <c r="G22">
+        <f t="shared" ca="1" si="5"/>
+        <v>38.690635913253558</v>
+      </c>
+      <c r="H22">
+        <f t="shared" ca="1" si="6"/>
+        <v>17.785700138641317</v>
+      </c>
+      <c r="I22">
+        <f t="shared" ca="1" si="7"/>
+        <v>122.00127305366755</v>
+      </c>
+      <c r="J22">
+        <f t="shared" ca="1" si="8"/>
+        <v>17.785700138641317</v>
+      </c>
+      <c r="K22">
+        <f t="shared" ca="1" si="9"/>
+        <v>81.114250073681262</v>
+      </c>
+      <c r="L22">
+        <f t="shared" ca="1" si="10"/>
+        <v>7.8431372549019605</v>
+      </c>
+      <c r="M22">
+        <f t="shared" ca="1" si="11"/>
+        <v>124.5591329439472</v>
+      </c>
+      <c r="N22">
+        <f t="shared" ca="1" si="12"/>
+        <v>1.3071895424836601</v>
+      </c>
+      <c r="O22">
+        <f t="shared" ca="1" si="13"/>
+        <v>72.404377318161991</v>
+      </c>
+      <c r="P22">
+        <f t="shared" ca="1" si="14"/>
+        <v>126.70275447831942</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>3000</v>
+      </c>
+      <c r="B23">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.41137555276431531</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ca="1" si="1"/>
+        <v>110.9392418580493</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ca="1" si="2"/>
+        <v>2.5600583428842544E-2</v>
+      </c>
+      <c r="E23">
+        <f t="shared" ca="1" si="3"/>
+        <v>102.84698979725741</v>
+      </c>
+      <c r="F23">
+        <f t="shared" ca="1" si="4"/>
+        <v>8.5371365928936654E-3</v>
+      </c>
+      <c r="G23">
+        <f t="shared" ca="1" si="5"/>
+        <v>45.354014826758082</v>
+      </c>
+      <c r="H23">
+        <f t="shared" ca="1" si="6"/>
+        <v>26.678550207961976</v>
+      </c>
+      <c r="I23">
+        <f t="shared" ca="1" si="7"/>
+        <v>121.0327711288613</v>
+      </c>
+      <c r="J23">
+        <f t="shared" ca="1" si="8"/>
+        <v>26.678550207961976</v>
+      </c>
+      <c r="K23">
+        <f t="shared" ca="1" si="9"/>
+        <v>76.920541615058454</v>
+      </c>
+      <c r="L23">
+        <f t="shared" ca="1" si="10"/>
+        <v>11.764705882352942</v>
+      </c>
+      <c r="M23">
+        <f t="shared" ca="1" si="11"/>
+        <v>121.11958056947213</v>
+      </c>
+      <c r="N23">
+        <f t="shared" ca="1" si="12"/>
+        <v>1.9607843137254901</v>
+      </c>
+      <c r="O23">
+        <f t="shared" ca="1" si="13"/>
+        <v>64.308684119281793</v>
+      </c>
+      <c r="P23">
+        <f t="shared" ca="1" si="14"/>
+        <v>124.32326064032651</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>4000</v>
+      </c>
+      <c r="B24">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.54850073701908708</v>
+      </c>
+      <c r="C24">
+        <f t="shared" ca="1" si="1"/>
+        <v>108.78815090172965</v>
+      </c>
+      <c r="D24">
+        <f t="shared" ca="1" si="2"/>
+        <v>3.4134111238456721E-2</v>
+      </c>
+      <c r="E24">
+        <f t="shared" ca="1" si="3"/>
+        <v>106.01554927405388</v>
+      </c>
+      <c r="F24">
+        <f t="shared" ca="1" si="4"/>
+        <v>1.1382848790524886E-2</v>
+      </c>
+      <c r="G24">
+        <f t="shared" ca="1" si="5"/>
+        <v>49.911756530984874</v>
+      </c>
+      <c r="H24">
+        <f t="shared" ca="1" si="6"/>
+        <v>35.571400277282635</v>
+      </c>
+      <c r="I24">
+        <f t="shared" ca="1" si="7"/>
+        <v>120.34560807751564</v>
+      </c>
+      <c r="J24">
+        <f t="shared" ca="1" si="8"/>
+        <v>35.571400277282635</v>
+      </c>
+      <c r="K24">
+        <f t="shared" ca="1" si="9"/>
+        <v>73.871138403833655</v>
+      </c>
+      <c r="L24">
+        <f t="shared" ca="1" si="10"/>
+        <v>15.686274509803921</v>
+      </c>
+      <c r="M24">
+        <f t="shared" ca="1" si="11"/>
+        <v>118.35680074706652</v>
+      </c>
+      <c r="N24">
+        <f t="shared" ca="1" si="12"/>
+        <v>2.6143790849673203</v>
+      </c>
+      <c r="O24">
+        <f t="shared" ca="1" si="13"/>
+        <v>54.813059169566415</v>
+      </c>
+      <c r="P24">
+        <f t="shared" ca="1" si="14"/>
+        <v>122.74952741482971</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>5000</v>
+      </c>
+      <c r="B25">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.68562592127385891</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ca="1" si="1"/>
+        <v>107.03607715245428</v>
+      </c>
+      <c r="D25">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.2667639048070909E-2</v>
+      </c>
+      <c r="E25">
+        <f t="shared" ca="1" si="3"/>
+        <v>108.02666972353258</v>
+      </c>
+      <c r="F25">
+        <f t="shared" ca="1" si="4"/>
+        <v>1.422856098815611E-2</v>
+      </c>
+      <c r="G25">
+        <f t="shared" ca="1" si="5"/>
+        <v>53.302410148240291</v>
+      </c>
+      <c r="H25">
+        <f t="shared" ca="1" si="6"/>
+        <v>44.464250346603293</v>
+      </c>
+      <c r="I25">
+        <f t="shared" ca="1" si="7"/>
+        <v>119.81260300597131</v>
+      </c>
+      <c r="J25">
+        <f t="shared" ca="1" si="8"/>
+        <v>44.464250346603293</v>
+      </c>
+      <c r="K25">
+        <f t="shared" ca="1" si="9"/>
+        <v>71.482860672187513</v>
+      </c>
+      <c r="L25">
+        <f t="shared" ca="1" si="10"/>
+        <v>19.607843137254903</v>
+      </c>
+      <c r="M25">
+        <f t="shared" ca="1" si="11"/>
+        <v>116.10561447221906</v>
+      </c>
+      <c r="N25">
+        <f t="shared" ca="1" si="12"/>
+        <v>3.2679738562091503</v>
+      </c>
+      <c r="O25">
+        <f t="shared" ca="1" si="13"/>
+        <v>47.109545111993036</v>
+      </c>
+      <c r="P25">
+        <f t="shared" ca="1" si="14"/>
+        <v>121.70176828373519</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>6000</v>
+      </c>
+      <c r="B26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.82275110552863062</v>
+      </c>
+      <c r="C26">
+        <f t="shared" ca="1" si="1"/>
+        <v>105.56544767802103</v>
+      </c>
+      <c r="D26">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.1201166857685089E-2</v>
+      </c>
+      <c r="E26">
+        <f t="shared" ca="1" si="3"/>
+        <v>109.34074907240158</v>
+      </c>
+      <c r="F26">
+        <f t="shared" ca="1" si="4"/>
+        <v>1.7074273185787331E-2</v>
+      </c>
+      <c r="G26">
+        <f t="shared" ca="1" si="5"/>
+        <v>55.947908859568699</v>
+      </c>
+      <c r="H26">
+        <f t="shared" ca="1" si="6"/>
+        <v>53.357100415923952</v>
+      </c>
+      <c r="I26">
+        <f t="shared" ca="1" si="7"/>
+        <v>119.37710615270939</v>
+      </c>
+      <c r="J26">
+        <f t="shared" ca="1" si="8"/>
+        <v>53.357100415923952</v>
+      </c>
+      <c r="K26">
+        <f t="shared" ca="1" si="9"/>
+        <v>69.522106473086154</v>
+      </c>
+      <c r="L26">
+        <f t="shared" ca="1" si="10"/>
+        <v>23.529411764705884</v>
+      </c>
+      <c r="M26">
+        <f t="shared" ca="1" si="11"/>
+        <v>114.22055677193839</v>
+      </c>
+      <c r="N26">
+        <f t="shared" ca="1" si="12"/>
+        <v>3.9215686274509802</v>
+      </c>
+      <c r="O26">
+        <f t="shared" ca="1" si="13"/>
+        <v>40.782720813122999</v>
+      </c>
+      <c r="P26">
+        <f t="shared" ca="1" si="14"/>
+        <v>120.9781405695459</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>7000</v>
+      </c>
+      <c r="B27">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.95987628978340234</v>
+      </c>
+      <c r="C27">
+        <f t="shared" ca="1" si="1"/>
+        <v>104.30107632452659</v>
+      </c>
+      <c r="D27">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.9734694667299269E-2</v>
+      </c>
+      <c r="E27">
+        <f t="shared" ca="1" si="3"/>
+        <v>110.20555244955658</v>
+      </c>
+      <c r="F27">
+        <f t="shared" ca="1" si="4"/>
+        <v>1.9919985383418552E-2</v>
+      </c>
+      <c r="G27">
+        <f t="shared" ca="1" si="5"/>
+        <v>58.075755587077353</v>
+      </c>
+      <c r="H27">
+        <f t="shared" ca="1" si="6"/>
+        <v>62.249950485244611</v>
+      </c>
+      <c r="I27">
+        <f t="shared" ca="1" si="7"/>
+        <v>119.00889880974103</v>
+      </c>
+      <c r="J27">
+        <f t="shared" ca="1" si="8"/>
+        <v>62.249950485244611</v>
+      </c>
+      <c r="K27">
+        <f t="shared" ca="1" si="9"/>
+        <v>67.859776103929335</v>
+      </c>
+      <c r="L27">
+        <f t="shared" ca="1" si="10"/>
+        <v>27.450980392156861</v>
+      </c>
+      <c r="M27">
+        <f t="shared" ca="1" si="11"/>
+        <v>112.60429611412546</v>
+      </c>
+      <c r="N27">
+        <f t="shared" ca="1" si="12"/>
+        <v>4.5751633986928102</v>
+      </c>
+      <c r="O27">
+        <f t="shared" ca="1" si="13"/>
+        <v>35.428627719065865</v>
+      </c>
+      <c r="P27">
+        <f t="shared" ca="1" si="14"/>
+        <v>120.45277307228518</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>8000</v>
+      </c>
+      <c r="B28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.0970014740381742</v>
+      </c>
+      <c r="C28">
+        <f t="shared" ca="1" si="1"/>
+        <v>103.19345406373432</v>
+      </c>
+      <c r="D28">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.8268222476913443E-2</v>
+      </c>
+      <c r="E28">
+        <f t="shared" ca="1" si="3"/>
+        <v>110.76773316785996</v>
+      </c>
+      <c r="F28">
+        <f t="shared" ca="1" si="4"/>
+        <v>2.2765697581049772E-2</v>
+      </c>
+      <c r="G28">
+        <f t="shared" ca="1" si="5"/>
+        <v>59.823355515639172</v>
+      </c>
+      <c r="H28">
+        <f t="shared" ca="1" si="6"/>
+        <v>71.14280055456527</v>
+      </c>
+      <c r="I28">
+        <f t="shared" ca="1" si="7"/>
+        <v>118.68994310136374</v>
+      </c>
+      <c r="J28">
+        <f t="shared" ca="1" si="8"/>
+        <v>71.14280055456527</v>
+      </c>
+      <c r="K28">
+        <f t="shared" ca="1" si="9"/>
+        <v>66.417344165834905</v>
+      </c>
+      <c r="L28">
+        <f t="shared" ca="1" si="10"/>
+        <v>31.372549019607842</v>
+      </c>
+      <c r="M28">
+        <f t="shared" ca="1" si="11"/>
+        <v>111.19193945392695</v>
+      </c>
+      <c r="N28">
+        <f t="shared" ca="1" si="12"/>
+        <v>5.2287581699346406</v>
+      </c>
+      <c r="O28">
+        <f t="shared" ca="1" si="13"/>
+        <v>30.789717380914801</v>
+      </c>
+      <c r="P28">
+        <f t="shared" ca="1" si="14"/>
+        <v>120.04914429883573</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>9000</v>
+      </c>
+      <c r="B29">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.2341266582929458</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ca="1" si="1"/>
+        <v>102.20863498719538</v>
+      </c>
+      <c r="D29">
+        <f t="shared" ca="1" si="2"/>
+        <v>7.6801750286527637E-2</v>
+      </c>
+      <c r="E29">
+        <f t="shared" ca="1" si="3"/>
+        <v>111.11965818848799</v>
+      </c>
+      <c r="F29">
+        <f t="shared" ca="1" si="4"/>
+        <v>2.5611409778680996E-2</v>
+      </c>
+      <c r="G29">
+        <f t="shared" ca="1" si="5"/>
+        <v>61.280427165667447</v>
+      </c>
+      <c r="H29">
+        <f t="shared" ca="1" si="6"/>
+        <v>80.035650623885928</v>
+      </c>
+      <c r="I29">
+        <f t="shared" ca="1" si="7"/>
+        <v>118.40860422790314</v>
+      </c>
+      <c r="J29">
+        <f t="shared" ca="1" si="8"/>
+        <v>80.035650623885928</v>
+      </c>
+      <c r="K29">
+        <f t="shared" ca="1" si="9"/>
+        <v>65.14358492579629</v>
+      </c>
+      <c r="L29">
+        <f t="shared" ca="1" si="10"/>
+        <v>35.294117647058826</v>
+      </c>
+      <c r="M29">
+        <f t="shared" ca="1" si="11"/>
+        <v>109.93887966429836</v>
+      </c>
+      <c r="N29">
+        <f t="shared" ca="1" si="12"/>
+        <v>5.882352941176471</v>
+      </c>
+      <c r="O29">
+        <f t="shared" ca="1" si="13"/>
+        <v>26.697657887688816</v>
+      </c>
+      <c r="P29">
+        <f t="shared" ca="1" si="14"/>
+        <v>119.72132642549448</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>10000</v>
+      </c>
+      <c r="B30">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.3712518425477178</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ca="1" si="1"/>
+        <v>101.32246260564992</v>
+      </c>
+      <c r="D30">
+        <f t="shared" ca="1" si="2"/>
+        <v>8.5335278096141817E-2</v>
+      </c>
+      <c r="E30">
+        <f ca="1">10*LOG10((($B$12*$B$9*$H$16*$H$15*(0.613*(10*D30)^4*((10*D30)^1.5+0.5)^-4))/(4*PI()*$B$15^2*(1-$B$7*COS($B$14))^4))/$B$17^2)</f>
+        <v>111.32211911502516</v>
+      </c>
+      <c r="F30">
+        <f t="shared" ca="1" si="4"/>
+        <v>2.845712197631222E-2</v>
+      </c>
+      <c r="G30">
+        <f t="shared" ca="1" si="5"/>
+        <v>62.508976847534647</v>
+      </c>
+      <c r="H30">
+        <f t="shared" ca="1" si="6"/>
+        <v>88.928500693206587</v>
+      </c>
+      <c r="I30">
+        <f t="shared" ca="1" si="7"/>
+        <v>118.15693802981943</v>
+      </c>
+      <c r="J30">
+        <f t="shared" ca="1" si="8"/>
+        <v>88.928500693206587</v>
+      </c>
+      <c r="K30">
+        <f t="shared" ca="1" si="9"/>
+        <v>64.003264234478593</v>
+      </c>
+      <c r="L30">
+        <f t="shared" ca="1" si="10"/>
+        <v>39.215686274509807</v>
+      </c>
+      <c r="M30">
+        <f t="shared" ca="1" si="11"/>
+        <v>108.81340529117922</v>
+      </c>
+      <c r="N30">
+        <f t="shared" ca="1" si="12"/>
+        <v>6.5359477124183005</v>
+      </c>
+      <c r="O30">
+        <f t="shared" ca="1" si="13"/>
+        <v>23.037110404610882</v>
+      </c>
+      <c r="P30">
+        <f t="shared" ca="1" si="14"/>
+        <v>119.44194371127141</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{268BB194-94B2-4982-A80B-F1F54D8DC0E8}">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
@@ -18262,12 +20171,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AD48"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AC43" sqref="AC43"/>
+    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5:AB34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18330,26 +20239,50 @@
       <c r="A5" t="s">
         <v>70</v>
       </c>
+      <c r="M5" t="s">
+        <v>128</v>
+      </c>
       <c r="N5" t="s">
         <v>129</v>
       </c>
+      <c r="O5" t="s">
+        <v>131</v>
+      </c>
       <c r="P5" t="s">
         <v>132</v>
       </c>
+      <c r="Q5" t="s">
+        <v>135</v>
+      </c>
       <c r="R5" t="s">
         <v>133</v>
       </c>
+      <c r="S5" t="s">
+        <v>137</v>
+      </c>
       <c r="T5" t="s">
         <v>109</v>
       </c>
+      <c r="U5" t="s">
+        <v>139</v>
+      </c>
       <c r="V5" t="s">
         <v>140</v>
       </c>
+      <c r="W5" t="s">
+        <v>142</v>
+      </c>
       <c r="X5" t="s">
         <v>120</v>
       </c>
+      <c r="Y5" t="s">
+        <v>144</v>
+      </c>
       <c r="Z5" t="s">
         <v>147</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>146</v>
       </c>
       <c r="AB5" t="s">
         <v>148</v>
@@ -18368,53 +20301,26 @@
       <c r="I6" t="s">
         <v>99</v>
       </c>
-      <c r="M6" t="s">
-        <v>128</v>
-      </c>
       <c r="N6" t="s">
         <v>130</v>
       </c>
-      <c r="O6" t="s">
-        <v>131</v>
-      </c>
       <c r="P6" t="s">
         <v>134</v>
       </c>
-      <c r="Q6" t="s">
-        <v>135</v>
-      </c>
       <c r="R6" t="s">
         <v>136</v>
       </c>
-      <c r="S6" t="s">
-        <v>137</v>
-      </c>
       <c r="T6" t="s">
         <v>138</v>
       </c>
-      <c r="U6" t="s">
-        <v>139</v>
-      </c>
       <c r="V6" t="s">
         <v>141</v>
       </c>
-      <c r="W6" t="s">
-        <v>142</v>
-      </c>
       <c r="X6" t="s">
         <v>143</v>
       </c>
-      <c r="Y6" t="s">
-        <v>144</v>
-      </c>
       <c r="Z6" t="s">
         <v>145</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>149</v>
       </c>
       <c r="AC6" t="s">
         <v>150</v>
@@ -21504,7 +23410,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AD48"/>
   <sheetViews>
@@ -24707,7 +26613,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AD48"/>
   <sheetViews>

</xml_diff>